<commit_message>
Replaced 4M12/1M divider by 3M9/953k divider to stay in JLCPCBs part lib
</commit_message>
<xml_diff>
--- a/BMS Slave Files/BatMeas5.3 Manufacturing Files/Assembly/batmeas-plc.xlsx
+++ b/BMS Slave Files/BatMeas5.3 Manufacturing Files/Assembly/batmeas-plc.xlsx
@@ -281,17 +281,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E128"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E49" activeCellId="0" sqref="E49"/>
+      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.1"/>
@@ -820,7 +820,7 @@
         <v>22.615</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>270</v>

</xml_diff>